<commit_message>
nu også med silica
</commit_message>
<xml_diff>
--- a/data/Pilot_scale/IC_data_pilot.xlsx
+++ b/data/Pilot_scale/IC_data_pilot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/Pilot_scale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="712" documentId="8_{529273BA-EBA1-4BB3-9FC2-78EA086EE824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42BBC27D-AB6D-450D-9E08-CAC3E7536859}"/>
+  <xr:revisionPtr revIDLastSave="765" documentId="8_{529273BA-EBA1-4BB3-9FC2-78EA086EE824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C023F46-DF23-4AA5-8820-9554AE5F9EA3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{A3B4B287-0889-4B6D-B999-70EA7A7FF5DD}"/>
+    <workbookView xWindow="3435" yWindow="2085" windowWidth="21600" windowHeight="11385" activeTab="7" xr2:uid="{A3B4B287-0889-4B6D-B999-70EA7A7FF5DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cl" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Mg" sheetId="7" r:id="rId5"/>
     <sheet name="K" sheetId="8" r:id="rId6"/>
     <sheet name="NO3" sheetId="9" r:id="rId7"/>
-    <sheet name="std" sheetId="2" r:id="rId8"/>
+    <sheet name="SiO2" sheetId="10" r:id="rId8"/>
+    <sheet name="std" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="29">
   <si>
     <t>Std 1 mg/l</t>
   </si>
@@ -7904,10 +7905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A805B470-D70E-48DE-BA3F-1B834C1F37C2}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8289,45 +8290,35 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <v>31.687213245561544</v>
-      </c>
-      <c r="F19">
-        <v>31.759026531019355</v>
-      </c>
-      <c r="G19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1">
         <v>5</v>
       </c>
       <c r="E20">
-        <v>26.145621384400563</v>
+        <v>31.687213245561544</v>
       </c>
       <c r="F20">
-        <v>26.321164971075209</v>
+        <v>31.759026531019355</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -8339,46 +8330,46 @@
         <v>3.2</v>
       </c>
       <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>26.145621384400563</v>
+      </c>
+      <c r="F21">
+        <v>26.321164971075209</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>3.2</v>
+      </c>
+      <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1">
-        <v>5</v>
-      </c>
-      <c r="E21">
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="E22">
         <v>29.522840614402558</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>29.532814681827251</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="1">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <v>38.539397566327551</v>
-      </c>
-      <c r="F22">
-        <v>38.539397566327551</v>
-      </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
       <c r="B23">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -8387,10 +8378,10 @@
         <v>5</v>
       </c>
       <c r="E23">
-        <v>39.309395571514067</v>
+        <v>38.539397566327551</v>
       </c>
       <c r="F23">
-        <v>39.31936963893876</v>
+        <v>38.539397566327551</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -8402,16 +8393,16 @@
         <v>0.5</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1">
         <v>5</v>
       </c>
       <c r="E24">
-        <v>33.841611809295834</v>
+        <v>39.309395571514067</v>
       </c>
       <c r="F24">
-        <v>33.835627368841017</v>
+        <v>39.31936963893876</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -8420,19 +8411,19 @@
         <v>18</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1">
         <v>5</v>
       </c>
       <c r="E25">
-        <v>35.557151406343507</v>
+        <v>33.841611809295834</v>
       </c>
       <c r="F25">
-        <v>35.59505286255736</v>
+        <v>33.835627368841017</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -8444,16 +8435,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1">
         <v>5</v>
       </c>
       <c r="E26">
-        <v>40.56014362657092</v>
+        <v>35.557151406343507</v>
       </c>
       <c r="F26">
-        <v>40.643925792938361</v>
+        <v>35.59505286255736</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -8462,22 +8453,21 @@
         <v>18</v>
       </c>
       <c r="B27">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27" s="1">
         <v>5</v>
       </c>
       <c r="E27">
-        <v>41.784959106323562</v>
+        <v>40.56014362657092</v>
       </c>
       <c r="F27">
-        <v>41.786953919808504</v>
+        <v>40.643925792938361</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -8487,37 +8477,38 @@
         <v>1.5</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1">
         <v>5</v>
       </c>
       <c r="E28">
-        <v>37.787352882505495</v>
+        <v>41.784959106323562</v>
       </c>
       <c r="F28">
-        <v>37.745461799321767</v>
+        <v>41.786953919808504</v>
       </c>
       <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1">
         <v>5</v>
       </c>
       <c r="E29">
-        <v>39.08797127468582</v>
-      </c>
-      <c r="F29" s="1">
-        <v>48.353879912228216</v>
+        <v>37.787352882505495</v>
+      </c>
+      <c r="F29">
+        <v>37.745461799321767</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -8529,16 +8520,16 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1">
         <v>5</v>
       </c>
       <c r="E30">
-        <v>40.43447037701975</v>
-      </c>
-      <c r="F30">
-        <v>40.452423698384202</v>
+        <v>39.08797127468582</v>
+      </c>
+      <c r="F30" s="1">
+        <v>48.353879912228216</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -8547,19 +8538,19 @@
         <v>18</v>
       </c>
       <c r="B31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1">
         <v>5</v>
       </c>
       <c r="E31">
-        <v>43.947336923997611</v>
+        <v>40.43447037701975</v>
       </c>
       <c r="F31">
-        <v>43.963295431877128</v>
+        <v>40.452423698384202</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -8571,16 +8562,16 @@
         <v>2.5</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32" s="1">
         <v>5</v>
       </c>
       <c r="E32">
-        <v>43.937362856572911</v>
+        <v>43.947336923997611</v>
       </c>
       <c r="F32">
-        <v>43.951326550967494</v>
+        <v>43.963295431877128</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -8588,20 +8579,20 @@
       <c r="A33" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="1">
-        <v>3.2</v>
+      <c r="B33">
+        <v>2.5</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33" s="1">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>44.001196888090966</v>
+        <v>43.937362856572911</v>
       </c>
       <c r="F33">
-        <v>43.979253939756639</v>
+        <v>43.951326550967494</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -8613,18 +8604,39 @@
         <v>3.2</v>
       </c>
       <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>44.001196888090966</v>
+      </c>
+      <c r="F34">
+        <v>43.979253939756639</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="1">
-        <v>5</v>
-      </c>
-      <c r="E34">
+      <c r="D35" s="1">
+        <v>5</v>
+      </c>
+      <c r="E35">
         <v>36.037901456213845</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>36.047875523638545</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8634,10 +8646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2F9E6A-338A-45F2-A659-0658D08F6933}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9029,17 +9041,11 @@
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>89.926989335520915</v>
-      </c>
-      <c r="F19" s="1">
-        <v>89.924254853705222</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -9047,19 +9053,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>98.190593382553985</v>
+        <v>89.926989335520915</v>
       </c>
       <c r="F20" s="1">
-        <v>99.41564123598576</v>
+        <v>89.924254853705222</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -9071,37 +9077,37 @@
         <v>3.2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
-        <v>40.944216570959803</v>
+        <v>98.190593382553985</v>
       </c>
       <c r="F21" s="1">
-        <v>42.390757451462946</v>
+        <v>99.41564123598576</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>10.26879956248291</v>
+        <v>40.944216570959803</v>
       </c>
       <c r="F22" s="1">
-        <v>10.290675417008476</v>
+        <v>42.390757451462946</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -9110,7 +9116,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -9119,10 +9125,10 @@
         <v>5</v>
       </c>
       <c r="E23" s="1">
-        <v>11.761826633852886</v>
+        <v>10.26879956248291</v>
       </c>
       <c r="F23" s="1">
-        <v>11.780968006562755</v>
+        <v>10.290675417008476</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -9134,16 +9140,16 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1">
-        <v>14.206453377085042</v>
+        <v>11.761826633852886</v>
       </c>
       <c r="F24" s="1">
-        <v>14.255674049767569</v>
+        <v>11.780968006562755</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -9152,19 +9158,19 @@
         <v>18</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>4.1298878862455561</v>
+        <v>14.206453377085042</v>
       </c>
       <c r="F25" s="1">
-        <v>4.1408258135083402</v>
+        <v>14.255674049767569</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -9176,16 +9182,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1">
-        <v>53.979491386382279</v>
+        <v>4.1298878862455561</v>
       </c>
       <c r="F26" s="1">
-        <v>53.957615531856717</v>
+        <v>4.1408258135083402</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -9194,19 +9200,19 @@
         <v>18</v>
       </c>
       <c r="B27" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>17.263604047033088</v>
+        <v>53.979491386382279</v>
       </c>
       <c r="F27" s="1">
-        <v>17.241728192507519</v>
+        <v>53.957615531856717</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -9218,16 +9224,16 @@
         <v>1.5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
-        <v>20.514902925895541</v>
+        <v>17.263604047033088</v>
       </c>
       <c r="F28" s="1">
-        <v>20.55592015313098</v>
+        <v>17.241728192507519</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -9236,19 +9242,19 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>13.036095159967187</v>
+        <v>20.514902925895541</v>
       </c>
       <c r="F29" s="1">
-        <v>13.07437790538693</v>
+        <v>20.55592015313098</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -9260,16 +9266,16 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E30" s="1">
-        <v>28.562482909488647</v>
+        <v>13.036095159967187</v>
       </c>
       <c r="F30" s="1">
-        <v>28.546076018594473</v>
+        <v>13.07437790538693</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -9278,19 +9284,19 @@
         <v>18</v>
       </c>
       <c r="B31" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>40.036368608148749</v>
+        <v>28.562482909488647</v>
       </c>
       <c r="F31" s="1">
-        <v>40.170358217117851</v>
+        <v>28.546076018594473</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -9302,16 +9308,16 @@
         <v>2.5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>37.154224774405243</v>
+        <v>40.036368608148749</v>
       </c>
       <c r="F32" s="1">
-        <v>36.981952420016405</v>
+        <v>40.170358217117851</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -9320,19 +9326,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>45.633852884878316</v>
+        <v>37.154224774405243</v>
       </c>
       <c r="F33" s="1">
-        <v>45.625649439431228</v>
+        <v>36.981952420016405</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -9344,18 +9350,38 @@
         <v>3.2</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>45.633852884878316</v>
+      </c>
+      <c r="F34" s="1">
+        <v>45.625649439431228</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
         <v>22.631391851244185</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>22.694284933005189</v>
       </c>
-      <c r="G34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9364,10 +9390,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E5C4B6-BC16-44C3-BBAE-0A09183A092F}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9735,7 +9761,7 @@
         <v>142.89121529358215</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -9743,16 +9769,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1">
-        <v>132.16294947655894</v>
-      </c>
-      <c r="F19" s="1">
-        <v>128.76285844333182</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -9760,19 +9777,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1">
-        <v>148.72189349112426</v>
+        <v>132.16294947655894</v>
       </c>
       <c r="F20" s="1">
-        <v>147.45653163404643</v>
+        <v>128.76285844333182</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -9783,36 +9800,36 @@
         <v>3.2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1">
-        <v>64.862084660901232</v>
+        <v>148.72189349112426</v>
       </c>
       <c r="F21" s="1">
-        <v>62.822940373236229</v>
+        <v>147.45653163404643</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22">
         <v>5</v>
       </c>
       <c r="E22" s="1">
-        <v>65.813381884387795</v>
+        <v>64.862084660901232</v>
       </c>
       <c r="F22" s="1">
-        <v>65.654073736913972</v>
+        <v>62.822940373236229</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -9820,7 +9837,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -9829,10 +9846,10 @@
         <v>5</v>
       </c>
       <c r="E23" s="1">
-        <v>70.283113336367776</v>
+        <v>65.813381884387795</v>
       </c>
       <c r="F23" s="1">
-        <v>71.757851615839783</v>
+        <v>65.654073736913972</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -9843,16 +9860,16 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24">
         <v>5</v>
       </c>
       <c r="E24" s="1">
-        <v>42.727355484751932</v>
+        <v>70.283113336367776</v>
       </c>
       <c r="F24" s="1">
-        <v>42.290395994538002</v>
+        <v>71.757851615839783</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -9860,19 +9877,19 @@
         <v>18</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1">
-        <v>23.496586253982702</v>
+        <v>42.727355484751932</v>
       </c>
       <c r="F25" s="1">
-        <v>22.97769685935366</v>
+        <v>42.290395994538002</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -9883,16 +9900,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1">
-        <v>78.189349112426029</v>
+        <v>23.496586253982702</v>
       </c>
       <c r="F26" s="1">
-        <v>77.593081474738284</v>
+        <v>22.97769685935366</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -9900,19 +9917,19 @@
         <v>18</v>
       </c>
       <c r="B27" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="E27" s="1">
-        <v>86.851160673645879</v>
+        <v>78.189349112426029</v>
       </c>
       <c r="F27" s="1">
-        <v>86.710059171597635</v>
+        <v>77.593081474738284</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -9923,16 +9940,16 @@
         <v>1.5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
       <c r="E28" s="1">
-        <v>53.009558488848427</v>
+        <v>86.851160673645879</v>
       </c>
       <c r="F28" s="1">
-        <v>52.754665452890301</v>
+        <v>86.710059171597635</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -9940,19 +9957,19 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E29" s="1">
-        <v>55.890760127446512</v>
+        <v>53.009558488848427</v>
       </c>
       <c r="F29" s="1">
-        <v>55.986345015930816</v>
+        <v>52.754665452890301</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -9963,16 +9980,16 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E30" s="1">
-        <v>62.422394173873464</v>
+        <v>55.890760127446512</v>
       </c>
       <c r="F30" s="1">
-        <v>62.631770596267636</v>
+        <v>55.986345015930816</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -9980,19 +9997,19 @@
         <v>18</v>
       </c>
       <c r="B31" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E31" s="1">
-        <v>68.694583522985894</v>
+        <v>62.422394173873464</v>
       </c>
       <c r="F31" s="1">
-        <v>68.298588984979517</v>
+        <v>62.631770596267636</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -10003,16 +10020,16 @@
         <v>2.5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1">
-        <v>82.085571233500218</v>
+        <v>68.694583522985894</v>
       </c>
       <c r="F32" s="1">
-        <v>81.716886663632224</v>
+        <v>68.298588984979517</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -10020,19 +10037,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1">
-        <v>74.288575329995453</v>
+        <v>82.085571233500218</v>
       </c>
       <c r="F33" s="1">
-        <v>73.687756030951292</v>
+        <v>81.716886663632224</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -10043,15 +10060,35 @@
         <v>3.2</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1">
+        <v>74.288575329995453</v>
+      </c>
+      <c r="F34" s="1">
+        <v>73.687756030951292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34">
-        <v>5</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1">
         <v>52.158397815202541</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>51.935366408739185</v>
       </c>
     </row>
@@ -10062,10 +10099,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7A271D-7927-42DB-A6AF-BBD6F7D577E7}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10433,7 +10470,7 @@
         <v>6.1257186661556151</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -10441,16 +10478,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>12.52280567267152</v>
-      </c>
-      <c r="F19" s="1">
-        <v>12.174013031812954</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -10458,19 +10486,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>6.2637025680337297</v>
+        <v>12.52280567267152</v>
       </c>
       <c r="F20" s="1">
-        <v>6.0298965120735906</v>
+        <v>12.174013031812954</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -10481,36 +10509,36 @@
         <v>3.2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
-        <v>10.709850517439632</v>
+        <v>6.2637025680337297</v>
       </c>
       <c r="F21" s="1">
-        <v>10.882330394787274</v>
+        <v>6.0298965120735906</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>2.0436949022614028</v>
+        <v>10.709850517439632</v>
       </c>
       <c r="F22" s="1">
-        <v>2.472978152548869</v>
+        <v>10.882330394787274</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -10518,7 +10546,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -10527,10 +10555,10 @@
         <v>5</v>
       </c>
       <c r="E23" s="1">
-        <v>2.9214258336527403</v>
+        <v>2.0436949022614028</v>
       </c>
       <c r="F23" s="1">
-        <v>2.9444231506324261</v>
+        <v>2.472978152548869</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -10541,16 +10569,16 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1">
-        <v>5.8535837485626674</v>
+        <v>2.9214258336527403</v>
       </c>
       <c r="F24" s="1">
-        <v>5.7155998466845537</v>
+        <v>2.9444231506324261</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -10558,19 +10586,19 @@
         <v>18</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>1.3652740513606745</v>
+        <v>5.8535837485626674</v>
       </c>
       <c r="F25" s="1">
-        <v>1.3691069375239555</v>
+        <v>5.7155998466845537</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -10581,16 +10609,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1">
-        <v>13.005749329244921</v>
+        <v>1.3652740513606745</v>
       </c>
       <c r="F26" s="1">
-        <v>13.04024530471445</v>
+        <v>1.3691069375239555</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -10598,19 +10626,19 @@
         <v>18</v>
       </c>
       <c r="B27" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>3.9984668455346868</v>
+        <v>13.005749329244921</v>
       </c>
       <c r="F27" s="1">
-        <v>4.1211192027596777</v>
+        <v>13.04024530471445</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -10621,16 +10649,16 @@
         <v>1.5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
-        <v>7.35990801073208</v>
+        <v>3.9984668455346868</v>
       </c>
       <c r="F28" s="1">
-        <v>7.3062476044461482</v>
+        <v>4.1211192027596777</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -10638,19 +10666,19 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>5.3438098888463008</v>
+        <v>7.35990801073208</v>
       </c>
       <c r="F29" s="1">
-        <v>5.5162897661939434</v>
+        <v>7.3062476044461482</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -10661,16 +10689,16 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1">
-        <v>9.0502108087389797</v>
+        <v>5.3438098888463008</v>
       </c>
       <c r="F30" s="1">
-        <v>8.9505557684936754</v>
+        <v>5.5162897661939434</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -10678,19 +10706,19 @@
         <v>18</v>
       </c>
       <c r="B31" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>8.9122269068608659</v>
+        <v>9.0502108087389797</v>
       </c>
       <c r="F31" s="1">
-        <v>8.9160597930241465</v>
+        <v>8.9505557684936754</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -10701,16 +10729,16 @@
         <v>2.5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>11.725565350709083</v>
+        <v>8.9122269068608659</v>
       </c>
       <c r="F32" s="1">
-        <v>11.599080107320813</v>
+        <v>8.9160597930241465</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -10718,19 +10746,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>9.5829819854350315</v>
+        <v>11.725565350709083</v>
       </c>
       <c r="F33" s="1">
-        <v>9.6098121885779992</v>
+        <v>11.599080107320813</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -10741,15 +10769,35 @@
         <v>3.2</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>9.5829819854350315</v>
+      </c>
+      <c r="F34" s="1">
+        <v>9.6098121885779992</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
         <v>8.1648141050210796</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>8.0613261786124948</v>
       </c>
     </row>
@@ -10760,10 +10808,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18253E7-7F77-46D2-BFE4-8D868396DD48}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11131,7 +11179,7 @@
         <v>3.4068469362441078</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -11139,16 +11187,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>3.5284048623170432</v>
-      </c>
-      <c r="F19" s="1">
-        <v>3.3076159761845698</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -11156,19 +11195,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>3.5631356983378817</v>
+        <v>3.5284048623170432</v>
       </c>
       <c r="F20" s="1">
-        <v>3.5656164723393697</v>
+        <v>3.3076159761845698</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -11179,40 +11218,44 @@
         <v>3.2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
-        <v>1.521458695112875</v>
+        <v>3.5631356983378817</v>
       </c>
       <c r="F21" s="1">
-        <v>1.516497147109898</v>
+        <v>3.5656164723393697</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.521458695112875</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.516497147109898</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -11231,10 +11274,10 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -11244,13 +11287,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -11263,33 +11306,33 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1.7943438352766061</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1.7000744232200444</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1.7943438352766061</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1.7000744232200444</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -11299,33 +11342,33 @@
         <v>1.5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1.3105929049863556</v>
-      </c>
-      <c r="F28" s="1">
-        <v>0.96824609278094775</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.3105929049863556</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.96824609278094775</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -11335,36 +11378,32 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1.2460927809476556</v>
-      </c>
-      <c r="F30" s="1">
-        <v>1.3924584470354748</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>1.0153807988092285</v>
+        <v>1.2460927809476556</v>
       </c>
       <c r="F31" s="1">
-        <v>1.055073182833044</v>
+        <v>1.3924584470354748</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -11375,16 +11414,16 @@
         <v>2.5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>1.6380550731828329</v>
+        <v>1.0153807988092285</v>
       </c>
       <c r="F32" s="1">
-        <v>1.7893822872736291</v>
+        <v>1.055073182833044</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -11392,19 +11431,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>1.0749193748449517</v>
+        <v>1.6380550731828329</v>
       </c>
       <c r="F33" s="1">
-        <v>1.1270156288762094</v>
+        <v>1.7893822872736291</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -11415,15 +11454,35 @@
         <v>3.2</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.0749193748449517</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.1270156288762094</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
         <v>1.3825353510295209</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>1.2039196229223517</v>
       </c>
     </row>
@@ -11434,10 +11493,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E163586A-34C6-4078-A748-B5EF04F6CDFB}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11805,7 +11864,7 @@
         <v>3.7729502452697967</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -11813,16 +11872,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>8.2789067974772248</v>
-      </c>
-      <c r="F19" s="1">
-        <v>7.7042747021723894</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -11830,19 +11880,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>4.1233356692361598</v>
+        <v>8.2789067974772248</v>
       </c>
       <c r="F20" s="1">
-        <v>4.0182200420462513</v>
+        <v>7.7042747021723894</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -11853,40 +11903,44 @@
         <v>3.2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
-        <v>3.9901892081289421</v>
+        <v>4.1233356692361598</v>
       </c>
       <c r="F21" s="1">
-        <v>3.7098808689558513</v>
+        <v>4.0182200420462513</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1">
-        <v>5</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3.9901892081289421</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3.7098808689558513</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -11905,33 +11959,33 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <v>2.8128941836019621</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2.5746320953048349</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2.8128941836019621</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2.5746320953048349</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -11941,36 +11995,32 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
-        <v>4.9292221443587954</v>
-      </c>
-      <c r="F26" s="1">
-        <v>4.7960756832515772</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>1.0399439383321654</v>
+        <v>4.9292221443587954</v>
       </c>
       <c r="F27" s="1">
-        <v>1.0119131044148564</v>
+        <v>4.7960756832515772</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -11981,16 +12031,16 @@
         <v>1.5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
-        <v>3.4505956552207424</v>
+        <v>1.0399439383321654</v>
       </c>
       <c r="F28" s="1">
-        <v>3.2193412754029436</v>
+        <v>1.0119131044148564</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -11998,19 +12048,19 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>1.3062368605466015</v>
+        <v>3.4505956552207424</v>
       </c>
       <c r="F29" s="1">
-        <v>1.1590749824807287</v>
+        <v>3.2193412754029436</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -12021,16 +12071,16 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1">
-        <v>3.9691660826909603</v>
+        <v>1.3062368605466015</v>
       </c>
       <c r="F30" s="1">
-        <v>3.744919411352488</v>
+        <v>1.1590749824807287</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -12038,19 +12088,19 @@
         <v>18</v>
       </c>
       <c r="B31" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>1.9439383321653818</v>
+        <v>3.9691660826909603</v>
       </c>
       <c r="F31" s="1">
-        <v>1.8037841625788364</v>
+        <v>3.744919411352488</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -12061,16 +12111,16 @@
         <v>2.5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>5.1885073580939034</v>
+        <v>1.9439383321653818</v>
       </c>
       <c r="F32" s="1">
-        <v>5.0273300630693765</v>
+        <v>1.8037841625788364</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -12078,19 +12128,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>1.9439383321653818</v>
+        <v>5.1885073580939034</v>
       </c>
       <c r="F33" s="1">
-        <v>1.9018920812894182</v>
+        <v>5.0273300630693765</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -12101,15 +12151,35 @@
         <v>3.2</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.9439383321653818</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.9018920812894182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="1">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
         <v>3.3524877365101617</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>3.2053258584442892</v>
       </c>
     </row>
@@ -12120,10 +12190,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F27A337-B24E-4765-A33B-7AAECDB37326}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12490,7 +12560,7 @@
         <v>3.6190305206463194</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -12498,16 +12568,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1.378456014362657</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.378456014362657</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -12515,19 +12576,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20">
         <v>5</v>
       </c>
       <c r="E20" s="1">
-        <v>3.719569120287253</v>
+        <v>1.378456014362657</v>
       </c>
       <c r="F20" s="1">
-        <v>3.6549371633752243</v>
+        <v>1.378456014362657</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -12538,36 +12599,36 @@
         <v>3.2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
-        <v>4.0319569120287246</v>
+        <v>3.719569120287253</v>
       </c>
       <c r="F21" s="1">
-        <v>3.9134649910233392</v>
+        <v>3.6549371633752243</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>1.6728904847396766</v>
+        <v>4.0319569120287246</v>
       </c>
       <c r="F22" s="1">
-        <v>1.6764811490125671</v>
+        <v>3.9134649910233392</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -12575,7 +12636,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -12584,10 +12645,10 @@
         <v>5</v>
       </c>
       <c r="E23" s="1">
-        <v>1.6549371633752241</v>
+        <v>1.6728904847396766</v>
       </c>
       <c r="F23" s="1">
-        <v>1.6549371633752241</v>
+        <v>1.6764811490125671</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -12598,16 +12659,16 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1">
-        <v>7.9673249551166965</v>
+        <v>1.6549371633752241</v>
       </c>
       <c r="F24" s="1">
-        <v>7.9924596050269283</v>
+        <v>1.6549371633752241</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -12615,19 +12676,19 @@
         <v>18</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>1.7806104129263913</v>
+        <v>7.9673249551166965</v>
       </c>
       <c r="F25" s="1">
-        <v>1.7842010771992818</v>
+        <v>7.9924596050269283</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -12638,16 +12699,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1">
-        <v>4.1612208258527827</v>
+        <v>1.7806104129263913</v>
       </c>
       <c r="F26" s="1">
-        <v>4.1001795332136446</v>
+        <v>1.7842010771992818</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -12655,19 +12716,19 @@
         <v>18</v>
       </c>
       <c r="B27" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>1.6046678635547575</v>
+        <v>4.1612208258527827</v>
       </c>
       <c r="F27" s="1">
-        <v>1.5938958707360862</v>
+        <v>4.1001795332136446</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -12678,16 +12739,16 @@
         <v>1.5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
-        <v>7.8308797127468566</v>
+        <v>1.6046678635547575</v>
       </c>
       <c r="F28" s="1">
-        <v>7.8201077199281848</v>
+        <v>1.5938958707360862</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -12695,19 +12756,19 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>1.4215439856373429</v>
+        <v>7.8308797127468566</v>
       </c>
       <c r="F29" s="1">
-        <v>1.7087971274685816</v>
+        <v>7.8201077199281848</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -12718,16 +12779,16 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1">
-        <v>4.4628366247755835</v>
+        <v>1.4215439856373429</v>
       </c>
       <c r="F30" s="1">
-        <v>4.4771992818671453</v>
+        <v>1.7087971274685816</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -12735,19 +12796,19 @@
         <v>18</v>
       </c>
       <c r="B31" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>1.4502692998204665</v>
+        <v>4.4628366247755835</v>
       </c>
       <c r="F31" s="1">
-        <v>1.4430879712746856</v>
+        <v>4.4771992818671453</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -12758,16 +12819,16 @@
         <v>2.5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>4.7680430879712743</v>
+        <v>1.4502692998204665</v>
       </c>
       <c r="F32" s="1">
-        <v>4.7500897666068225</v>
+        <v>1.4430879712746856</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -12775,19 +12836,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="1">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>1.4179533213644524</v>
+        <v>4.7680430879712743</v>
       </c>
       <c r="F33" s="1">
-        <v>1.4179533213644524</v>
+        <v>4.7500897666068225</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -12798,15 +12859,35 @@
         <v>3.2</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.4179533213644524</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.4179533213644524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
         <v>7.6369838420107712</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>7.6441651705565512</v>
       </c>
     </row>
@@ -12816,6 +12897,650 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611BE9C8-98E7-482D-9BCD-F14F6130479D}">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>84.2</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>93.2</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>89.8</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>61.7</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>93.6</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>97.4</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>63.9</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>99.8</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>103</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>68</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>105</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>110.6</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>126.8</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>113.4</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>81.5</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>149.80000000000001</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>132.80000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>93.4</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>157.6</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>64</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>59.8</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>61.4</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>71.8</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>62.4</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>76</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>82.8</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>61.2</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75C754A-D74F-41EE-8888-ED859D942A8F}">
   <dimension ref="A1:F128"/>
   <sheetViews>

</xml_diff>